<commit_message>
uploaded the output files
</commit_message>
<xml_diff>
--- a/Project Outputs for AQM with ESP32-C3/BOM/Bill of Materials-AQM with ESP32-C3.xlsx
+++ b/Project Outputs for AQM with ESP32-C3/BOM/Bill of Materials-AQM with ESP32-C3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="5715" windowHeight="6735"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AQM with ESP3" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="218">
+  <si>
+    <t>Designator</t>
+  </si>
   <si>
     <t>Comment</t>
   </si>
   <si>
+    <t>Mfr. Part #</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Designator</t>
-  </si>
-  <si>
     <t>Footprint</t>
   </si>
   <si>
@@ -39,25 +45,22 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Mfr. Part #</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
     <t>LCSC Part #</t>
   </si>
   <si>
-    <t>Value</t>
+    <t>A1, A2</t>
   </si>
   <si>
     <t>IC1</t>
   </si>
   <si>
-    <t>75dB@(120Hz) 1A 1.25V@(1A) ±125?@(Tj) Fixed 3.3V~3.3V Positive 1 20V SOT-89 Linear Voltage Regulators (LDO) ROHS</t>
-  </si>
-  <si>
-    <t>A1, A2</t>
+    <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t>YONGYUTAI</t>
+  </si>
+  <si>
+    <t>75dB@(120Hz) 1A 1.25V@(1A) ±125℃@(Tj) Fixed 3.3V~3.3V Positive 1 20V SOT-89 Linear Voltage Regulators (LDO) ROHS</t>
   </si>
   <si>
     <t>SOT89-150P350X150-3N</t>
@@ -66,193 +69,196 @@
     <t>IC?</t>
   </si>
   <si>
-    <t>AMS1117-3.3</t>
-  </si>
-  <si>
-    <t>YONGYUTAI</t>
-  </si>
-  <si>
     <t>C2904742</t>
   </si>
   <si>
+    <t>B1</t>
+  </si>
+  <si>
     <t>10D561K</t>
   </si>
   <si>
+    <t>Hongzhi Elec</t>
+  </si>
+  <si>
     <t>920V 42.3J 180pF@1kHz 460V 350V 504V~616V 2.5kA Plugin Varistors ROHS</t>
   </si>
   <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>Hongzhi Elec</t>
-  </si>
-  <si>
     <t>C113236</t>
   </si>
   <si>
+    <t>B2</t>
+  </si>
+  <si>
     <t>UU9.8Y-10MH</t>
   </si>
   <si>
-    <t>10mH@1kHz 1.2O 2 500mA 50V Plugin Common Mode Filters ROHS</t>
-  </si>
-  <si>
-    <t>B2</t>
+    <t>FH (Guangdong Fenghua Advanced Tech)</t>
+  </si>
+  <si>
+    <t>10mH@1kHz 1.2Ω 2 500mA 50V Plugin Common Mode Filters ROHS</t>
   </si>
   <si>
     <t>UU98Y10MH</t>
   </si>
   <si>
-    <t>FH (Guangdong Fenghua Advanced Tech)</t>
-  </si>
-  <si>
     <t>C75192</t>
   </si>
   <si>
+    <t>B3</t>
+  </si>
+  <si>
     <t>3296X-1-103</t>
   </si>
   <si>
-    <t>±10% 10kO Plugin Variable Resistors/Potentiometers ROHS</t>
-  </si>
-  <si>
-    <t>B3</t>
+    <t>BOCHEN(Chengdu Guosheng Tech)</t>
+  </si>
+  <si>
+    <t>±10% 10kΩ Plugin Variable Resistors/Potentiometers ROHS</t>
   </si>
   <si>
     <t>3296X1223LF</t>
   </si>
   <si>
-    <t>BOCHEN(Chengdu Guosheng Tech)</t>
-  </si>
-  <si>
     <t>C118955</t>
   </si>
   <si>
+    <t>B4</t>
+  </si>
+  <si>
     <t>ESP32-C3-WROOM-02-N4</t>
   </si>
   <si>
+    <t>Espressif Systems</t>
+  </si>
+  <si>
     <t>WiFi Modules (802.11) (Engineering Samples) SMD module, ESP32-C3, 4MB SPI flash, PCB antenna, -40 C +85 C</t>
   </si>
   <si>
-    <t>B4</t>
-  </si>
-  <si>
     <t>ESP32C3WROOM02N4</t>
   </si>
   <si>
-    <t>Espressif Systems</t>
-  </si>
-  <si>
     <t>C2934560</t>
   </si>
   <si>
+    <t>C1</t>
+  </si>
+  <si>
     <t>0.1uF</t>
   </si>
   <si>
-    <t>0.1uF ±10% -40?~+110? X2 275VAC Radial Leaded,P=15mm Suppression Capacitors ROHS</t>
-  </si>
-  <si>
-    <t>C1</t>
+    <t>X2-104K-275VAC</t>
+  </si>
+  <si>
+    <t>NDF</t>
+  </si>
+  <si>
+    <t>X2 100nF ±10% 275V Plugin,P=15mm Suppression Capacitors ROHS</t>
   </si>
   <si>
     <t>MPX-104K275VAC-C-D2</t>
   </si>
   <si>
-    <t>CORETONG</t>
-  </si>
-  <si>
-    <t>C3249976</t>
+    <t/>
+  </si>
+  <si>
+    <t>C914484</t>
+  </si>
+  <si>
+    <t>C2</t>
   </si>
   <si>
     <t>220uF</t>
   </si>
   <si>
-    <t>-40?~+85? 2000hrs@85? 220uF 10mm 16V 8mm 215mA@120Hz ±20% SMD,D8xL10mm Aluminum Electrolytic Capacitors - SMD ROHS</t>
-  </si>
-  <si>
-    <t>C2</t>
+    <t>UUR1C221MNL1GS</t>
+  </si>
+  <si>
+    <t>Nichicon</t>
+  </si>
+  <si>
+    <t>-40℃~+85℃ 2000hrs@85℃ 220uF 10mm 16V 8mm 215mA@120Hz ±20% SMD,D8xL10mm Aluminum Electrolytic Capacitors - SMD ROHS</t>
   </si>
   <si>
     <t>CAPAE830X1050N</t>
   </si>
   <si>
-    <t>UUR1C221MNL1GS</t>
-  </si>
-  <si>
-    <t>Nichicon</t>
-  </si>
-  <si>
     <t>C445237</t>
   </si>
   <si>
+    <t>C3, C5</t>
+  </si>
+  <si>
     <t>22uF</t>
   </si>
   <si>
+    <t>GRM219R61C226ME15L</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
     <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0805, 22uF, X5R, 15%, 20%, 16V</t>
   </si>
   <si>
-    <t>C3, C5</t>
-  </si>
-  <si>
     <t>FP-GRM219-0_2-0_15-IPC_A</t>
   </si>
   <si>
     <t>CMP-06035-056251-1</t>
   </si>
   <si>
-    <t>GRM219R61C226ME15L</t>
-  </si>
-  <si>
-    <t>Murata Electronics</t>
-  </si>
-  <si>
     <t>C162295</t>
   </si>
   <si>
+    <t>C4, C6, C7</t>
+  </si>
+  <si>
     <t>10uF</t>
   </si>
   <si>
+    <t>CL05A106MQ5NUNC</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
     <t>6.3V 10uF X5R ±20% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t>C4, C6, C7</t>
-  </si>
-  <si>
-    <t>CL05A106MQ5NUNC</t>
-  </si>
-  <si>
-    <t>Samsung Electro-Mechanics</t>
-  </si>
-  <si>
     <t>C15525</t>
   </si>
   <si>
+    <t>C8</t>
+  </si>
+  <si>
     <t>100nF</t>
   </si>
   <si>
+    <t>CL05B104KO5NNNC</t>
+  </si>
+  <si>
     <t>X7R 100nF 16V ±10% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>CAPC1050X55X23ML05T13</t>
   </si>
   <si>
     <t>CMP-2000-05439-1</t>
   </si>
   <si>
-    <t>CL05B104KO5NNNC</t>
-  </si>
-  <si>
     <t>C1525</t>
   </si>
   <si>
+    <t>C9</t>
+  </si>
+  <si>
     <t>1uF</t>
   </si>
   <si>
-    <t>X5R 10V 1uF ±10% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
-  </si>
-  <si>
-    <t>C9</t>
+    <t>CL05A105KP5NNNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X5R 10V 1uF ±10% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
     <t>FP-CL511-IPC_C</t>
@@ -261,133 +267,133 @@
     <t>CMP-13271-001936-1</t>
   </si>
   <si>
-    <t>CL05A105KP5NNNC</t>
-  </si>
-  <si>
     <t>C14445</t>
   </si>
   <si>
+    <t>C10, C11</t>
+  </si>
+  <si>
     <t>12pF</t>
   </si>
   <si>
+    <t>CL10C120JB8NNNC</t>
+  </si>
+  <si>
     <t>50V 12pF C0G ±5% 0603 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t>C10, C11</t>
-  </si>
-  <si>
     <t>CAPC1608X90X30LL10T20</t>
   </si>
   <si>
     <t>CMP-2000-06098-1</t>
   </si>
   <si>
-    <t>CL10C120JB8NNNC</t>
-  </si>
-  <si>
     <t>C38523</t>
   </si>
   <si>
+    <t>D1</t>
+  </si>
+  <si>
     <t>Display</t>
   </si>
   <si>
     <t>Header, 4-Pin</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>HDR1X4</t>
   </si>
   <si>
     <t>Header 4</t>
   </si>
   <si>
+    <t>F1</t>
+  </si>
+  <si>
     <t>S6125-M2-0.5A</t>
   </si>
   <si>
+    <t>SART(Nanjing Sart Tech)</t>
+  </si>
+  <si>
     <t>SMD Fuses ROHS</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
     <t>CAPC6125X25N</t>
   </si>
   <si>
-    <t>SART(Nanjing Sart Tech)</t>
-  </si>
-  <si>
     <t>C845172</t>
   </si>
   <si>
+    <t>J1, J2, J3, J4, J5</t>
+  </si>
+  <si>
     <t>5004</t>
   </si>
   <si>
+    <t>Keystone</t>
+  </si>
+  <si>
     <t>PC TEST POINT MINIATURE YELLOW</t>
   </si>
   <si>
-    <t>J1, J2, J3, J4, J5</t>
-  </si>
-  <si>
     <t>FP-5004-MFG</t>
   </si>
   <si>
     <t>CMP-2000-05575-2</t>
   </si>
   <si>
-    <t>Keystone</t>
-  </si>
-  <si>
     <t>C2906762</t>
   </si>
   <si>
+    <t>J6</t>
+  </si>
+  <si>
     <t>10118192-0001LF</t>
   </si>
   <si>
+    <t>Amphenol ICC</t>
+  </si>
+  <si>
     <t>Single Port 5 Contact Horizontal Right Angle Shielded Micro B USB 2.0 Connector</t>
   </si>
   <si>
-    <t>J6</t>
-  </si>
-  <si>
     <t>AMPHENOL_10118192-0001LF</t>
   </si>
   <si>
-    <t>Amphenol ICC</t>
-  </si>
-  <si>
     <t>C132564</t>
   </si>
   <si>
+    <t>P1</t>
+  </si>
+  <si>
     <t>AC suppy</t>
   </si>
   <si>
+    <t>1729128</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
     <t>13.5A 400V Green Straight pin 5.08mm 1 2 Plugin,P=5.08mm Screw terminal ROHS</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>PHOE-1729128-2_V</t>
   </si>
   <si>
     <t>CMP-2000-05815-1</t>
   </si>
   <si>
-    <t>1729128</t>
-  </si>
-  <si>
-    <t>Phoenix Contact</t>
-  </si>
-  <si>
     <t>C91153</t>
   </si>
   <si>
+    <t>P2</t>
+  </si>
+  <si>
     <t>uv lamp</t>
   </si>
   <si>
-    <t>P2</t>
+    <t>P3</t>
   </si>
   <si>
     <t>Header 3</t>
@@ -396,19 +402,19 @@
     <t>Header, 3-Pin</t>
   </si>
   <si>
-    <t>P3</t>
-  </si>
-  <si>
     <t>HDR1X3</t>
   </si>
   <si>
+    <t>P4</t>
+  </si>
+  <si>
     <t>Hum/Tem Sensor</t>
   </si>
   <si>
     <t>Si7021 Header, 4-Pin</t>
   </si>
   <si>
-    <t>P4</t>
+    <t>P5</t>
   </si>
   <si>
     <t>CO2/VOC sensor</t>
@@ -417,34 +423,34 @@
     <t>SGP30 Header, 4-Pin</t>
   </si>
   <si>
-    <t>P5</t>
+    <t>P6</t>
   </si>
   <si>
     <t>CH2O sensor</t>
   </si>
   <si>
+    <t>ZE08-CH2O</t>
+  </si>
+  <si>
+    <t>Zhengzhou Winsen Elec Tech</t>
+  </si>
+  <si>
     <t>- Sensor Modules ROHS</t>
   </si>
   <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>ZE08-CH2O</t>
-  </si>
-  <si>
-    <t>Zhengzhou Winsen Elec Tech</t>
-  </si>
-  <si>
     <t>C141344</t>
   </si>
   <si>
+    <t>P7</t>
+  </si>
+  <si>
     <t>CO sensor</t>
   </si>
   <si>
     <t>MQ7 Header, 4-Pin</t>
   </si>
   <si>
-    <t>P7</t>
+    <t>P8</t>
   </si>
   <si>
     <t>O3 sensor</t>
@@ -453,106 +459,109 @@
     <t>MQ131 Header, 4-Pin</t>
   </si>
   <si>
-    <t>P8</t>
+    <t>P9</t>
   </si>
   <si>
     <t>PMS5003</t>
   </si>
   <si>
+    <t>Beijing Plantower</t>
+  </si>
+  <si>
     <t>PMS5003 Sensor Modules ROHS</t>
   </si>
   <si>
-    <t>P9</t>
-  </si>
-  <si>
     <t>HDR1X6</t>
   </si>
   <si>
     <t>Header 6</t>
   </si>
   <si>
-    <t>Beijing Plantower</t>
-  </si>
-  <si>
     <t>C91431</t>
   </si>
   <si>
+    <t>P10</t>
+  </si>
+  <si>
     <t>5V FAN</t>
   </si>
   <si>
     <t>Header, 2-Pin</t>
   </si>
   <si>
-    <t>P10</t>
-  </si>
-  <si>
     <t>HDR1X2</t>
   </si>
   <si>
     <t>Header 2</t>
   </si>
   <si>
+    <t>P11, P12</t>
+  </si>
+  <si>
     <t>Header 9</t>
   </si>
   <si>
     <t>Header, 9-Pin</t>
   </si>
   <si>
-    <t>P11, P12</t>
-  </si>
-  <si>
     <t>HDR1X9</t>
   </si>
   <si>
+    <t>Q1</t>
+  </si>
+  <si>
     <t>2SD313</t>
   </si>
   <si>
+    <t>Jiangsu Changjing Electronics Technology Co., Ltd.</t>
+  </si>
+  <si>
     <t>NPN Transistor, TO-220</t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
     <t>TO304P498X1010X2089-3P</t>
   </si>
   <si>
-    <t>Jiangsu Changjing Electronics Technology Co., Ltd.</t>
-  </si>
-  <si>
     <t>C3031919</t>
   </si>
   <si>
+    <t>R1, R2, R4, R5, R6, R7, R10, R12, R13, R14, R16, R17</t>
+  </si>
+  <si>
     <t>0R</t>
   </si>
   <si>
+    <t>RC0402FR-070RL</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
     <t>RES SMD 0 OHM JUMPER 1/16W 0402</t>
   </si>
   <si>
-    <t>R1, R2, R4, R5, R6, R7, R10, R12, R13, R14, R16, R17</t>
-  </si>
-  <si>
     <t>FP-RC0402-0_4-IPC_A</t>
   </si>
   <si>
     <t>CMP-2002-07342-2</t>
   </si>
   <si>
-    <t>RC0402FR-070RL</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
     <t>C106231</t>
   </si>
   <si>
+    <t>R3</t>
+  </si>
+  <si>
     <t>470Ω</t>
   </si>
   <si>
-    <t>100mW Thick Film Resistors 75V ±100ppm/? ±1% -55?~+155? 470O 0603 Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>R3</t>
+    <t>RC0603FR-07470RL</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>100mW Thick Film Resistors 75V ±100ppm/℃ ±1% -55℃~+155℃ 470Ω 0603 Chip Resistor - Surface Mount ROHS</t>
   </si>
   <si>
     <t>RESC1608X55X25LL10T15</t>
@@ -561,25 +570,19 @@
     <t>CMP-1659-00035-2</t>
   </si>
   <si>
-    <t>RC0603FR-07470RL</t>
-  </si>
-  <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
     <t>C114669</t>
   </si>
   <si>
-    <t>470O</t>
+    <t>R8, R9, R11</t>
   </si>
   <si>
     <t>10kΩ</t>
   </si>
   <si>
-    <t>50V 10kO Thick Film Resistors 62.5mW ±1% -55?~+155? ±100ppm/? 0402 Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>R8, R9, R11</t>
+    <t>RC0402FR-0710KL</t>
+  </si>
+  <si>
+    <t>50V 10kΩ Thick Film Resistors 62.5mW ±1% -55℃~+155℃ ±100ppm/℃ 0402 Chip Resistor - Surface Mount ROHS</t>
   </si>
   <si>
     <t>RESC1005X40X25LL05T10</t>
@@ -588,91 +591,85 @@
     <t>CMP-2002-07353-1</t>
   </si>
   <si>
-    <t>RC0402FR-0710KL</t>
-  </si>
-  <si>
     <t>C60490</t>
   </si>
   <si>
-    <t>10kO</t>
+    <t>S1</t>
   </si>
   <si>
     <t>Switch</t>
   </si>
   <si>
-    <t>Surface Mount 50mA DPDT 3.2mm 12V 9.1mm 12V 3.55mm 50mA 10000 SMDSplicing Rectangular columnar -40?~+85? Black SMD Slide Switches ROHS</t>
-  </si>
-  <si>
-    <t>S1</t>
+    <t>SK-3245S-L1-A</t>
+  </si>
+  <si>
+    <t>XKB Connectivity</t>
+  </si>
+  <si>
+    <t>Surface Mount 50mA DPDT 3.2mm 12V 9.1mm 12V 3.55mm 50mA 10000 SMDSplicing Rectangular columnar -40℃~+85℃ Black SMD Slide Switches ROHS</t>
   </si>
   <si>
     <t>SK3245SL1A</t>
   </si>
   <si>
-    <t>SK-3245S-L1-A</t>
-  </si>
-  <si>
-    <t>XKB Connectivity</t>
-  </si>
-  <si>
     <t>C405951</t>
   </si>
   <si>
+    <t>S2, S3, S4</t>
+  </si>
+  <si>
     <t>TL1105AF160Q</t>
   </si>
   <si>
+    <t>E-Switch</t>
+  </si>
+  <si>
     <t>6mm 1.4mm Round Button 50mA Straight 6mm SPST 12V Plugin,6x6mm Tactile Switches ROHS</t>
   </si>
   <si>
-    <t>S2, S3, S4</t>
-  </si>
-  <si>
-    <t>E-Switch</t>
-  </si>
-  <si>
     <t>C273465</t>
   </si>
   <si>
+    <t>U1</t>
+  </si>
+  <si>
     <t>HLK-10M05</t>
   </si>
   <si>
+    <t>HI-LINK</t>
+  </si>
+  <si>
     <t>5V 2A 90VAC~265VAC 1 120V~350V Isolated Regulated 10W AC-DC 80% Plugin Power Modules ROHS</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>FP-HLK-10M05-MFG</t>
   </si>
   <si>
     <t>CMP-218581-000001-1</t>
   </si>
   <si>
-    <t>HI-LINK</t>
-  </si>
-  <si>
     <t>C403745</t>
   </si>
   <si>
+    <t>Y1</t>
+  </si>
+  <si>
     <t>32.768kHz</t>
   </si>
   <si>
-    <t>-40?~+85? 32.768kHz 12.5pF 70kO ±20ppm SMD3215-2P Crystals ROHS</t>
-  </si>
-  <si>
-    <t>Y1</t>
+    <t>ABS07-32.768KHZ-T</t>
+  </si>
+  <si>
+    <t>Abracon LLC</t>
+  </si>
+  <si>
+    <t>-40℃~+85℃ 32.768kHz 12.5pF 70kΩ ±20ppm SMD3215-2P Crystals ROHS</t>
   </si>
   <si>
     <t>FP-ABS07-MFG</t>
   </si>
   <si>
     <t>CMP-0447-00001-4</t>
-  </si>
-  <si>
-    <t>ABS07-32.768KHZ-T</t>
-  </si>
-  <si>
-    <t>Abracon LLC</t>
   </si>
   <si>
     <t>C130253</t>
@@ -805,13 +802,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1133,17 +1130,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="10" width="16.5703125" customWidth="1"/>
+    <col min="1" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1171,414 +1167,384 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="4">
-        <v>2</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4">
+        <v>2</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="4">
-        <v>1</v>
+      <c r="F7" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="4">
+        <v>59</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="4">
         <v>2</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="I9" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="4">
-        <v>3</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="4">
+        <v>3</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="4">
-        <v>1</v>
+      <c r="F11" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="4">
-        <v>1</v>
+      <c r="F12" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="4">
         <v>2</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>96</v>
@@ -1587,28 +1553,27 @@
         <v>97</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" s="4">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>102</v>
@@ -1619,26 +1584,25 @@
       <c r="E16" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="4">
         <v>5</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="I16" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>109</v>
@@ -1647,238 +1611,229 @@
         <v>110</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="4">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20" s="4">
-        <v>1</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C21" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
       <c r="E21" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F21" s="4">
-        <v>1</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21" s="4">
+        <v>1</v>
+      </c>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
       <c r="E22" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="4">
-        <v>1</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G22" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1</v>
+      </c>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="4">
-        <v>1</v>
-      </c>
       <c r="G23" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C24" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="4">
+        <v>1</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="4">
-        <v>1</v>
-      </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="4">
+        <v>1</v>
+      </c>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>147</v>
@@ -1889,74 +1844,71 @@
       <c r="E26" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="4">
-        <v>1</v>
+      <c r="F26" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I26" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="4">
+        <v>1</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C27" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G27" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" s="4">
+      <c r="F28" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="4">
         <v>2</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>163</v>
@@ -1965,87 +1917,80 @@
         <v>164</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F29" s="4">
-        <v>1</v>
+        <v>165</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F30" s="4">
+        <v>172</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H30" s="4">
         <v>12</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="I30" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F31" s="4">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="I31" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="H31" s="4">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>184</v>
       </c>
@@ -2056,153 +2001,144 @@
         <v>186</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="F32" s="4">
-        <v>3</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="I32" s="3" t="s">
+      <c r="H32" s="4">
+        <v>3</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="J32" s="7" t="s">
+    </row>
+    <row r="33" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="B33" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F33" s="4">
-        <v>1</v>
-      </c>
       <c r="G33" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="H33" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="I33" s="3" t="s">
+    </row>
+    <row r="34" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="B34" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F34" s="4">
-        <v>3</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="4">
+        <v>3</v>
+      </c>
+      <c r="I34" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="I34" s="3" t="s">
+    </row>
+    <row r="35" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="B35" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F35" s="4">
-        <v>1</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="4">
+        <v>1</v>
+      </c>
+      <c r="I35" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="I35" s="3" t="s">
+    </row>
+    <row r="36" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="B36" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="E36" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="F36" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="F36" s="10">
-        <v>1</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H36" s="10">
+        <v>1</v>
+      </c>
+      <c r="I36" s="11" t="s">
         <v>217</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="27" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="23" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>